<commit_message>
quantidade de mp no resumo e tipo de chapa no template
</commit_message>
<xml_diff>
--- a/GERAR OP SERRA.xlsx
+++ b/GERAR OP SERRA.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>ORDEM DE PRODUÇÃO - SERRA</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>OS-489</t>
+  </si>
+  <si>
+    <t>TIPO MP</t>
   </si>
   <si>
     <t>Matéria-prima:</t>
@@ -104,7 +107,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -127,6 +130,12 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -136,12 +145,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -226,6 +229,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -276,21 +294,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -307,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -349,21 +352,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="5" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="5" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -372,28 +375,25 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="8" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="9" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="8" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="9" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -710,13 +710,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="30" width="20.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="31" width="52.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="31" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="31" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="31" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="31" width="36.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="31" width="37.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="29" width="20.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="30" width="52.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="30" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="30" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="30" width="15.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="30" width="36.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="30" width="37.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="25.125">
@@ -758,51 +758,55 @@
       <c r="C4" s="11"/>
       <c r="D4" s="12"/>
       <c r="E4" s="13"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="F4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="14">
+        <v>8.99999999999998</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="23.25">
       <c r="A5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
+      <c r="B5" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
       <c r="F5" s="16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="23.25">
       <c r="A6" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="18">
         <v>6000</v>
       </c>
       <c r="C6" s="19"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
       <c r="F6" s="16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G6" s="17"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="24">
       <c r="A7" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="19"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
       <c r="F7" s="16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G7" s="17">
         <f>B6-(C10*D10)</f>
@@ -819,154 +823,154 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
       <c r="A9" s="22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="60">
       <c r="A10" s="25" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="26"/>
-      <c r="C10" s="27">
+      <c r="C10" s="14">
         <v>8.99999999999998</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="14">
         <v>660</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="27">
         <v>1475.999999999997</v>
       </c>
-      <c r="F10" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="29" t="s">
+      <c r="F10" s="28" t="s">
         <v>19</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="60">
       <c r="A11" s="25"/>
       <c r="B11" s="26"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29" t="s">
-        <v>19</v>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="60">
       <c r="A12" s="25"/>
       <c r="B12" s="26"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="75">
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="60">
       <c r="A13" s="25"/>
       <c r="B13" s="26"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29" t="s">
-        <v>19</v>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="75">
       <c r="A14" s="25"/>
       <c r="B14" s="26"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29" t="s">
-        <v>19</v>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="75">
       <c r="A15" s="25"/>
       <c r="B15" s="26"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29" t="s">
-        <v>19</v>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="75">
       <c r="A16" s="25"/>
       <c r="B16" s="26"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29" t="s">
-        <v>19</v>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="75">
       <c r="A17" s="25"/>
       <c r="B17" s="26"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29" t="s">
-        <v>19</v>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="75">
       <c r="A18" s="25"/>
       <c r="B18" s="26"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29" t="s">
-        <v>19</v>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="75">
       <c r="A19" s="25"/>
       <c r="B19" s="26"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29" t="s">
-        <v>19</v>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="75">
       <c r="A20" s="25"/>
       <c r="B20" s="26"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29" t="s">
-        <v>19</v>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>